<commit_message>
ebola stacked running wo exceptions
</commit_message>
<xml_diff>
--- a/analysis/results-summary.xlsx
+++ b/analysis/results-summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>random</t>
   </si>
@@ -40,15 +40,9 @@
     <t>0.31(0.03)</t>
   </si>
   <si>
-    <t>0.46(0.02)</t>
-  </si>
-  <si>
     <t>0.42(0.01)</t>
   </si>
   <si>
-    <t>0.38(0.01)</t>
-  </si>
-  <si>
     <t>0.47(0.01)</t>
   </si>
   <si>
@@ -64,9 +58,6 @@
     <t>0.04(0.01)</t>
   </si>
   <si>
-    <t>0.29(0.02)</t>
-  </si>
-  <si>
     <t>0.39(0.02)</t>
   </si>
   <si>
@@ -104,6 +95,33 @@
   </si>
   <si>
     <t>0.24(0.02)</t>
+  </si>
+  <si>
+    <t>0.03(0.01)</t>
+  </si>
+  <si>
+    <t>0.40(0.02)</t>
+  </si>
+  <si>
+    <t>0.43(0.01)</t>
+  </si>
+  <si>
+    <t>Ebola</t>
+  </si>
+  <si>
+    <t>0.17(0.01)</t>
+  </si>
+  <si>
+    <t>0.21(0.005)</t>
+  </si>
+  <si>
+    <t>0.16(0.004)</t>
+  </si>
+  <si>
+    <t>0.36(0.003)</t>
+  </si>
+  <si>
+    <t>0.45(0.02)</t>
   </si>
 </sst>
 </file>
@@ -482,17 +500,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -520,22 +538,22 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -543,13 +561,13 @@
         <v>0.5</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -558,7 +576,7 @@
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -566,22 +584,22 @@
         <v>0.75</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -589,27 +607,27 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -637,7 +655,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -645,7 +663,7 @@
         <v>0.5</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -653,7 +671,7 @@
         <v>0.75</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -661,7 +679,46 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add one tsep mb nn
</commit_message>
<xml_diff>
--- a/analysis/results-summary.xlsx
+++ b/analysis/results-summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
   <si>
     <t>random</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>0.76(0.008)</t>
+  </si>
+  <si>
+    <t>0.03(0.006)</t>
   </si>
 </sst>
 </file>
@@ -563,7 +566,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,6 +867,9 @@
       <c r="C22" t="s">
         <v>44</v>
       </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
       <c r="I22" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
update nn mb results
</commit_message>
<xml_diff>
--- a/analysis/results-summary.xlsx
+++ b/analysis/results-summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>random</t>
   </si>
@@ -185,6 +185,30 @@
   </si>
   <si>
     <t>0.03(0.006)</t>
+  </si>
+  <si>
+    <t>mb two step</t>
+  </si>
+  <si>
+    <t>0.20(0.026)</t>
+  </si>
+  <si>
+    <t>0.59(0.009)</t>
+  </si>
+  <si>
+    <t>0.61(0.009)</t>
+  </si>
+  <si>
+    <t>0.63(0.011)</t>
+  </si>
+  <si>
+    <t>0.60(0.010)</t>
+  </si>
+  <si>
+    <t>0.75(0.009)</t>
+  </si>
+  <si>
+    <t>0.75(0.010)</t>
   </si>
 </sst>
 </file>
@@ -563,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,7 +824,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>34</v>
       </c>
@@ -826,12 +850,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -856,8 +880,11 @@
       <c r="I21" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -873,8 +900,11 @@
       <c r="I22" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.5</v>
       </c>
@@ -884,11 +914,17 @@
       <c r="C23" t="s">
         <v>46</v>
       </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
       <c r="I23" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.75</v>
       </c>
@@ -898,11 +934,17 @@
       <c r="C24" t="s">
         <v>48</v>
       </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
       <c r="I24" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -912,8 +954,14 @@
       <c r="C25" t="s">
         <v>50</v>
       </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
       <c r="I25" t="s">
         <v>51</v>
+      </c>
+      <c r="J25" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add results for lattice 2step
</commit_message>
<xml_diff>
--- a/analysis/results-summary.xlsx
+++ b/analysis/results-summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="68">
   <si>
     <t>random</t>
   </si>
@@ -209,6 +209,15 @@
   </si>
   <si>
     <t>0.75(0.010)</t>
+  </si>
+  <si>
+    <t>0.35(0.02)</t>
+  </si>
+  <si>
+    <t>mf two step prefit (1e5 on lattice data)</t>
+  </si>
+  <si>
+    <t>0.45(0.012)</t>
   </si>
 </sst>
 </file>
@@ -587,20 +596,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -625,8 +634,14 @@
       <c r="I2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -654,8 +669,14 @@
       <c r="I3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.5</v>
       </c>
@@ -681,7 +702,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.75</v>
       </c>
@@ -707,7 +728,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -733,12 +754,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -761,7 +782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
@@ -769,7 +790,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.5</v>
       </c>
@@ -777,7 +798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.75</v>
       </c>
@@ -785,7 +806,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -793,12 +814,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -824,7 +845,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>34</v>
       </c>
@@ -850,12 +871,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -883,8 +904,11 @@
       <c r="J21" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
@@ -904,7 +928,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.5</v>
       </c>
@@ -924,7 +948,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.75</v>
       </c>
@@ -944,7 +968,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
debug contiuation, add results
</commit_message>
<xml_diff>
--- a/analysis/results-summary.xlsx
+++ b/analysis/results-summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="206">
   <si>
     <t>random</t>
   </si>
@@ -599,21 +599,6 @@
   </si>
   <si>
     <t>one step continuation</t>
-  </si>
-  <si>
-    <t>0.54(0.012)</t>
-  </si>
-  <si>
-    <t>0.49(0.014)</t>
-  </si>
-  <si>
-    <t>0.46(0.021)</t>
-  </si>
-  <si>
-    <t>0.36(0.018)</t>
-  </si>
-  <si>
-    <t>0.45(0.016)</t>
   </si>
   <si>
     <t>one step mse averaged new model</t>
@@ -1035,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1102,7 +1087,7 @@
         <v>174</v>
       </c>
       <c r="R2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="S2" t="s">
         <v>182</v>
@@ -1223,16 +1208,13 @@
         <v>175</v>
       </c>
       <c r="R4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="S4" t="s">
         <v>175</v>
       </c>
       <c r="T4" t="s">
-        <v>203</v>
-      </c>
-      <c r="V4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1279,13 +1261,10 @@
         <v>179</v>
       </c>
       <c r="R5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="S5" t="s">
         <v>181</v>
-      </c>
-      <c r="V5" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1340,9 +1319,6 @@
       <c r="T6" t="s">
         <v>176</v>
       </c>
-      <c r="V6" t="s">
-        <v>198</v>
-      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1517,7 +1493,7 @@
         <v>174</v>
       </c>
       <c r="R21" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="S21" t="s">
         <v>182</v>
@@ -1574,19 +1550,16 @@
         <v>180</v>
       </c>
       <c r="R22" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="S22" t="s">
         <v>187</v>
       </c>
       <c r="T22" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="U22" t="s">
         <v>191</v>
-      </c>
-      <c r="V22" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
@@ -1631,7 +1604,7 @@
         <v>181</v>
       </c>
       <c r="R23" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="S23" t="s">
         <v>188</v>
@@ -1641,9 +1614,6 @@
       </c>
       <c r="U23" t="s">
         <v>191</v>
-      </c>
-      <c r="V23" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.25">
@@ -1688,7 +1658,7 @@
         <v>178</v>
       </c>
       <c r="R24" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="S24" t="s">
         <v>189</v>
@@ -1742,19 +1712,16 @@
         <v>170</v>
       </c>
       <c r="R25" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="S25" t="s">
         <v>185</v>
       </c>
       <c r="T25" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="U25" t="s">
         <v>192</v>
-      </c>
-      <c r="V25" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>